<commit_message>
Novas alterações no app
</commit_message>
<xml_diff>
--- a/Dados.xlsx
+++ b/Dados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Lista_de_Parâmetros" sheetId="6" r:id="rId1"/>
@@ -23,9 +23,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Custos!$A$1:$D$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lista_de_Parâmetros!$A$1:$F$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Parametros!$A$1:$G$10</definedName>
-    <definedName name="Ano_Inicial">Configs!$D$2:$D$2</definedName>
+    <definedName name="Ano_Inicial">Configs!$C$2:$C$2</definedName>
     <definedName name="Anos_a_Serem_Simulados">Configs!$A$2</definedName>
-    <definedName name="CategoriaSAT">Configs!$C$2:$C$2</definedName>
+    <definedName name="CategoriaSAT">Configs!#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="128">
   <si>
     <t>Ano</t>
   </si>
@@ -48,9 +48,6 @@
     <t>FolhadePagamento</t>
   </si>
   <si>
-    <t>CategoriaSAT</t>
-  </si>
-  <si>
     <t>AnoInicial</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Parametro4</t>
   </si>
   <si>
-    <t>CNPJ</t>
-  </si>
-  <si>
     <t>Iniciativa1</t>
   </si>
   <si>
@@ -111,12 +105,6 @@
     <t>IniciativasTestadas</t>
   </si>
   <si>
-    <t>Vacina da Gripe</t>
-  </si>
-  <si>
-    <t>Novo Equipamento</t>
-  </si>
-  <si>
     <t>Descrição</t>
   </si>
   <si>
@@ -171,36 +159,6 @@
     <t>SemIniciativa</t>
   </si>
   <si>
-    <t>NomeInicativa1</t>
-  </si>
-  <si>
-    <t>NomeIniciativa2</t>
-  </si>
-  <si>
-    <t>NomeIniciativa3</t>
-  </si>
-  <si>
-    <t>NomeIniciativa4</t>
-  </si>
-  <si>
-    <t>NomeIniciativa5</t>
-  </si>
-  <si>
-    <t>NomeIniciativa6</t>
-  </si>
-  <si>
-    <t>NomeIniciativa7</t>
-  </si>
-  <si>
-    <t>NomeIniciativa8</t>
-  </si>
-  <si>
-    <t>NomeIniciativa9</t>
-  </si>
-  <si>
-    <t>NomeIniciativa10</t>
-  </si>
-  <si>
     <t>Iniciativa3</t>
   </si>
   <si>
@@ -226,9 +184,6 @@
   </si>
   <si>
     <t>TodasIniciativas</t>
-  </si>
-  <si>
-    <t>TestarIniciativasEmConjunto?</t>
   </si>
   <si>
     <t>Categoria</t>
@@ -889,78 +844,78 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +929,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -986,24 +943,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C2" s="12">
         <v>2017</v>
@@ -1014,10 +971,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C3" s="12">
         <v>2018</v>
@@ -1028,10 +985,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C4" s="12">
         <v>2017</v>
@@ -1042,10 +999,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C5" s="12">
         <v>2018</v>
@@ -1074,120 +1031,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="2">
         <v>1000</v>
       </c>
-      <c r="C2" s="2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>2017</v>
       </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
       <c r="E2">
-        <v>123412321</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1231,38 +1125,38 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="M1" s="9" t="str">
         <f>"CustoMedioMulta_Lei1"</f>
         <v>CustoMedioMulta_Lei1</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1280,20 +1174,20 @@
       <c r="D2" s="5">
         <v>750</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="5" t="e">
         <f>F2*C2</f>
-        <v>153000</v>
-      </c>
-      <c r="F2" s="7">
+        <v>#REF!</v>
+      </c>
+      <c r="F2" s="7" t="e">
         <f>G2*H2</f>
-        <v>0.06</v>
+        <v>#REF!</v>
       </c>
       <c r="G2" s="6">
         <v>0.02</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="e">
         <f>CategoriaSAT</f>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="I2" s="14">
         <v>8</v>
@@ -1330,20 +1224,20 @@
         <f>ROUND(D2*1.08,2)</f>
         <v>810</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="5" t="e">
         <f t="shared" ref="E3" si="2">F3*C3</f>
-        <v>153000</v>
-      </c>
-      <c r="F3" s="7">
+        <v>#REF!</v>
+      </c>
+      <c r="F3" s="7" t="e">
         <f t="shared" ref="F3" si="3">G3*H3</f>
-        <v>0.06</v>
+        <v>#REF!</v>
       </c>
       <c r="G3" s="6">
         <v>0.02</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="e">
         <f t="shared" ref="H3" si="4">CategoriaSAT</f>
-        <v>3</v>
+        <v>#REF!</v>
       </c>
       <c r="I3" s="14">
         <v>8</v>
@@ -1439,18 +1333,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2" t="b">
         <f>TRUE</f>
@@ -1463,7 +1357,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <f>TRUE</f>
@@ -1476,7 +1370,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B4" t="b">
         <f>FALSE</f>
@@ -1489,7 +1383,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B5" t="b">
         <f>FALSE</f>
@@ -1502,7 +1396,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B6" t="b">
         <f>FALSE</f>
@@ -1515,7 +1409,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B7" t="b">
         <f>FALSE</f>
@@ -1528,7 +1422,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B8" t="b">
         <f>FALSE</f>
@@ -1541,7 +1435,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B9" t="b">
         <f>FALSE</f>
@@ -1554,7 +1448,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B10" t="b">
         <f>FALSE</f>
@@ -1567,7 +1461,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B11" t="b">
         <f>FALSE</f>
@@ -1580,7 +1474,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B12" t="b">
         <f>FALSE</f>
@@ -1593,7 +1487,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B13" t="b">
         <f>FALSE</f>
@@ -1617,7 +1511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1633,33 +1527,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>5.0000000000000001E-3</v>
@@ -1671,15 +1565,15 @@
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>5.0000000000000001E-3</v>
@@ -1689,15 +1583,15 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>5.0000000000000001E-3</v>
@@ -1707,15 +1601,15 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>5.0000000000000001E-3</v>
@@ -1725,15 +1619,15 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1743,15 +1637,15 @@
         <v>0.05</v>
       </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>0.4</v>
@@ -1761,15 +1655,15 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>0.3</v>
@@ -1779,15 +1673,15 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>0.2</v>
@@ -1797,15 +1691,15 @@
         <v>2E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C10">
         <v>0.1</v>
@@ -1815,15 +1709,15 @@
         <v>1E-3</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <f>C2-0.002</f>
@@ -1836,15 +1730,15 @@
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:C14" si="1">C3-0.002</f>
@@ -1855,15 +1749,15 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -1874,15 +1768,15 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -1893,15 +1787,15 @@
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <f>C6-1</f>
@@ -1912,15 +1806,15 @@
         <v>0.04</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -1930,15 +1824,15 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C17">
         <v>0.3</v>
@@ -1948,15 +1842,15 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="G17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C18">
         <v>0.2</v>
@@ -1966,15 +1860,15 @@
         <v>2E-3</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -1984,15 +1878,15 @@
         <v>1E-3</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C20">
         <v>1000</v>
@@ -2002,15 +1896,15 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C21">
         <v>1000</v>
@@ -2020,15 +1914,15 @@
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C22">
         <v>5</v>
@@ -2038,15 +1932,15 @@
         <v>0.05</v>
       </c>
       <c r="G22" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C23">
         <v>5</v>
@@ -2056,15 +1950,15 @@
         <v>0.05</v>
       </c>
       <c r="G23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2074,15 +1968,15 @@
         <v>0.02</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2092,15 +1986,15 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2110,15 +2004,15 @@
         <v>0.02</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2128,15 +2022,15 @@
         <v>0.01</v>
       </c>
       <c r="G27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C28">
         <v>0.5</v>
@@ -2146,15 +2040,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <v>0.5</v>
@@ -2164,15 +2058,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>10</v>
@@ -2182,15 +2076,15 @@
         <v>0.1</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C31">
         <v>10</v>
@@ -2200,15 +2094,15 @@
         <v>0.1</v>
       </c>
       <c r="G31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C32">
         <v>0.1</v>
@@ -2218,15 +2112,15 @@
         <v>1E-3</v>
       </c>
       <c r="G32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C33">
         <v>0.1</v>
@@ -2236,7 +2130,7 @@
         <v>1E-3</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2250,8 +2144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2263,18 +2157,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -2286,10 +2180,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="C3" t="b">
         <f>TRUE</f>
@@ -2298,10 +2192,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C4" t="b">
         <f>TRUE</f>
@@ -2310,10 +2204,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C5" t="b">
         <f>TRUE</f>
@@ -2322,10 +2216,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C6" t="b">
         <f>TRUE</f>
@@ -2334,10 +2228,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C7" t="b">
         <f>TRUE</f>
@@ -2346,10 +2240,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C8" t="b">
         <f>TRUE</f>
@@ -2358,10 +2252,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C9" t="b">
         <f>TRUE</f>
@@ -2370,10 +2264,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C10" t="b">
         <f>TRUE</f>
@@ -2382,10 +2276,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C11" t="b">
         <f>TRUE</f>
@@ -2394,7 +2288,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -2406,10 +2300,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C13" t="b">
         <f>FALSE</f>
@@ -2418,10 +2312,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C14" t="b">
         <f>FALSE</f>
@@ -2430,10 +2324,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C15" t="b">
         <f>FALSE</f>
@@ -2442,10 +2336,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C16" t="b">
         <f>FALSE</f>
@@ -2454,10 +2348,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C17" t="b">
         <f>FALSE</f>
@@ -2466,10 +2360,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C18" t="b">
         <f>FALSE</f>
@@ -2478,10 +2372,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="C19" t="b">
         <f>FALSE</f>
@@ -2490,10 +2384,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C20" t="b">
         <f>FALSE</f>
@@ -2502,10 +2396,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C21" t="b">
         <f>TRUE</f>
@@ -2514,7 +2408,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -2526,10 +2420,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" t="b">
         <f>FALSE</f>
@@ -2538,10 +2432,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" t="b">
         <f>FALSE</f>
@@ -2550,10 +2444,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C25" t="b">
         <f>TRUE</f>
@@ -2562,10 +2456,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C26" t="b">
         <f>FALSE</f>
@@ -2574,10 +2468,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C27" t="b">
         <f>FALSE</f>
@@ -2586,10 +2480,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C28" t="b">
         <f>FALSE</f>
@@ -2598,10 +2492,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C29" t="b">
         <f>FALSE</f>
@@ -2610,10 +2504,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C30" t="b">
         <f>FALSE</f>
@@ -2622,7 +2516,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B31" t="str">
         <f>"NumeroMultasAPriori_"&amp;D31</f>
@@ -2633,12 +2527,12 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B32" t="str">
         <f>"CustoMedioMulta_"&amp;D32</f>
@@ -2649,12 +2543,12 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B33" t="str">
         <f>"Atendimento_"&amp;D33</f>
@@ -2665,15 +2559,15 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C34" t="b">
         <f>FALSE</f>
@@ -2682,10 +2576,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C35" t="b">
         <f>FALSE</f>
@@ -2694,74 +2588,74 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2787,233 +2681,233 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B24" t="str">
         <f>"NumeroMultas_"&amp;C24</f>
         <v>NumeroMultas_Lei1</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -3039,55 +2933,55 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -3107,22 +3001,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>